<commit_message>
fixing command descriptions for cmos1
</commit_message>
<xml_diff>
--- a/commands/cmos1/cmos1_command_deck.xlsx
+++ b/commands/cmos1/cmos1_command_deck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi-4matter/foxsi4-commands/commands/cmos1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C615F99-7E64-6C4C-9DB1-273FBF26C5A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E802CE-4E87-BA43-B76B-ED029AD0DD20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17900" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="301">
   <si>
     <t>R=1/W=0</t>
   </si>
@@ -925,6 +925,18 @@
   </si>
   <si>
     <t>0x218</t>
+  </si>
+  <si>
+    <t>shuts down CMOS operating system</t>
+  </si>
+  <si>
+    <t>enables shutdown, reboot, and remove all data commands</t>
+  </si>
+  <si>
+    <t>reboots CMOS operating system</t>
+  </si>
+  <si>
+    <t>deletes all stored image data</t>
   </si>
 </sst>
 </file>
@@ -1427,10 +1439,10 @@
   <dimension ref="A1:AC85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B64" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B55" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A80" sqref="A80:A85"/>
+      <selection pane="bottomRight" activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -5209,7 +5221,7 @@
         <v>70</v>
       </c>
       <c r="AC43" t="s">
-        <v>82</v>
+        <v>298</v>
       </c>
     </row>
     <row r="44" spans="1:29" ht="16" x14ac:dyDescent="0.2">
@@ -5299,7 +5311,7 @@
         <v>70</v>
       </c>
       <c r="AC44" t="s">
-        <v>82</v>
+        <v>297</v>
       </c>
     </row>
     <row r="45" spans="1:29" ht="16" x14ac:dyDescent="0.2">
@@ -5388,6 +5400,9 @@
       <c r="AB45" t="s">
         <v>70</v>
       </c>
+      <c r="AC45" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="46" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="19" t="s">
@@ -5474,6 +5489,9 @@
       </c>
       <c r="AB46" t="s">
         <v>70</v>
+      </c>
+      <c r="AC46" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="47" spans="1:29" ht="16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
make all spw write commands reply; cdte and cmos get readall command
1. all SpaceWire write commands now have instruction field == 0x7d
   (verify and reply) populated, and reply length for write commands is
0x08 (data length of write reply).
2. all cdte (including cdtede) and cmos get a read_all_hk command to
   collect housekeeping data in a single block for downlink. All these
blocks are sub-MTU (single packet transmittable).
</commit_message>
<xml_diff>
--- a/commands/cmos1/cmos1_command_deck.xlsx
+++ b/commands/cmos1/cmos1_command_deck.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi-4matter/foxsi4-commands/commands/cmos1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E802CE-4E87-BA43-B76B-ED029AD0DD20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66346D7-8988-D74D-99E7-F5014444A5CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17900" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
+    <workbookView xWindow="20" yWindow="760" windowWidth="30220" windowHeight="17880" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
   <sheets>
     <sheet name="all_systems" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="298">
   <si>
     <t>R=1/W=0</t>
   </si>
@@ -597,9 +597,6 @@
     <t>0x0000008c</t>
   </si>
   <si>
-    <t>0x75</t>
-  </si>
-  <si>
     <t>start CMOS setup (first stops, then inits, then trains, then sets exposure).</t>
   </si>
   <si>
@@ -609,105 +606,6 @@
     <t>set_exposure_192</t>
   </si>
   <si>
-    <t>set_exposure_value_02</t>
-  </si>
-  <si>
-    <t>set_exposure_value_03</t>
-  </si>
-  <si>
-    <t>set_exposure_value_04</t>
-  </si>
-  <si>
-    <t>set_exposure_value_05</t>
-  </si>
-  <si>
-    <t>set_exposure_value_06</t>
-  </si>
-  <si>
-    <t>set_exposure_value_07</t>
-  </si>
-  <si>
-    <t>set_exposure_value_08</t>
-  </si>
-  <si>
-    <t>set_exposure_value_09</t>
-  </si>
-  <si>
-    <t>set_exposure_value_10</t>
-  </si>
-  <si>
-    <t>set_exposure_value_11</t>
-  </si>
-  <si>
-    <t>set_exposure_value_12</t>
-  </si>
-  <si>
-    <t>set_exposure_value_13</t>
-  </si>
-  <si>
-    <t>set_exposure_value_14</t>
-  </si>
-  <si>
-    <t>set_exposure_value_15</t>
-  </si>
-  <si>
-    <t>set_exposure_value_16</t>
-  </si>
-  <si>
-    <t>set_exposure_value_17</t>
-  </si>
-  <si>
-    <t>set_exposure_value_18</t>
-  </si>
-  <si>
-    <t>set_exposure_value_19</t>
-  </si>
-  <si>
-    <t>set_exposure_value_20</t>
-  </si>
-  <si>
-    <t>set_exposure_value_21</t>
-  </si>
-  <si>
-    <t>set_exposure_value_0a</t>
-  </si>
-  <si>
-    <t>set_exposure_value_0b</t>
-  </si>
-  <si>
-    <t>set_exposure_value_0c</t>
-  </si>
-  <si>
-    <t>set_exposure_value_0d</t>
-  </si>
-  <si>
-    <t>set_exposure_value_0e</t>
-  </si>
-  <si>
-    <t>set_exposure_value_0f</t>
-  </si>
-  <si>
-    <t>set_exposure_value_1a</t>
-  </si>
-  <si>
-    <t>set_exposure_value_1b</t>
-  </si>
-  <si>
-    <t>set_exposure_value_1c</t>
-  </si>
-  <si>
-    <t>set_exposure_value_1d</t>
-  </si>
-  <si>
-    <t>set_exposure_value_1e</t>
-  </si>
-  <si>
-    <t>set_exposure_value_1f</t>
-  </si>
-  <si>
-    <t>set quick look mode and photon counting mode exposure time to 192 for CMOS camera</t>
-  </si>
-  <si>
     <t>0x00000030</t>
   </si>
   <si>
@@ -717,21 +615,6 @@
     <t>0x021085f0</t>
   </si>
   <si>
-    <t>set quick look mode and photon counting mode exposure time to 0x02 for CMOS sensor</t>
-  </si>
-  <si>
-    <t>set quick look mode and photon counting mode exposure time to 0x03 for CMOS sensor</t>
-  </si>
-  <si>
-    <t>set quick look mode and photon counting mode exposure time to 0x04 for CMOS sensor</t>
-  </si>
-  <si>
-    <t>set quick look mode and photon counting mode exposure time to 0x05 for CMOS sensor</t>
-  </si>
-  <si>
-    <t>set quick look mode and photon counting mode exposure time to 0x06 for CMOS sensor</t>
-  </si>
-  <si>
     <t>0x031085f0</t>
   </si>
   <si>
@@ -750,162 +633,33 @@
     <t>0x081085f0</t>
   </si>
   <si>
-    <t>0x091085f0</t>
-  </si>
-  <si>
     <t>0x0a1085f0</t>
   </si>
   <si>
     <t>0x0b1085f0</t>
   </si>
   <si>
-    <t>0x0c1085f0</t>
-  </si>
-  <si>
     <t>0x0d1085f0</t>
   </si>
   <si>
-    <t>0x0e1085f0</t>
-  </si>
-  <si>
     <t>0x0f1085f0</t>
   </si>
   <si>
-    <t>0x111085f0</t>
-  </si>
-  <si>
-    <t>0x101085f0</t>
-  </si>
-  <si>
     <t>0x121085f0</t>
   </si>
   <si>
-    <t>0x131085f0</t>
-  </si>
-  <si>
     <t>0x141085f0</t>
   </si>
   <si>
-    <t>0x151085f0</t>
-  </si>
-  <si>
-    <t>0x161085f0</t>
-  </si>
-  <si>
-    <t>0x171085f0</t>
-  </si>
-  <si>
     <t>0x181085f0</t>
   </si>
   <si>
-    <t>0x191085f0</t>
-  </si>
-  <si>
-    <t>0x1a1085f0</t>
-  </si>
-  <si>
     <t>0x1b1085f0</t>
   </si>
   <si>
-    <t>0x1c1085f0</t>
-  </si>
-  <si>
-    <t>0x1d1085f0</t>
-  </si>
-  <si>
-    <t>0x1e1085f0</t>
-  </si>
-  <si>
     <t>0x1f1085f0</t>
   </si>
   <si>
-    <t>0x201085f0</t>
-  </si>
-  <si>
-    <t>0x211085f0</t>
-  </si>
-  <si>
-    <t>set quick look mode and photon counting mode exposure time to 0x07 for CMOS sensor</t>
-  </si>
-  <si>
-    <t>set quick look mode and photon counting mode exposure time to 0x08 for CMOS sensor</t>
-  </si>
-  <si>
-    <t>set quick look mode and photon counting mode exposure time to 0x09 for CMOS sensor</t>
-  </si>
-  <si>
-    <t>set quick look mode and photon counting mode exposure time to 0x0a for CMOS sensor</t>
-  </si>
-  <si>
-    <t>set quick look mode and photon counting mode exposure time to 0x0b for CMOS sensor</t>
-  </si>
-  <si>
-    <t>set quick look mode and photon counting mode exposure time to 0x0c for CMOS sensor</t>
-  </si>
-  <si>
-    <t>set quick look mode and photon counting mode exposure time to 0x0d for CMOS sensor</t>
-  </si>
-  <si>
-    <t>set quick look mode and photon counting mode exposure time to 0x0e for CMOS sensor</t>
-  </si>
-  <si>
-    <t>set quick look mode and photon counting mode exposure time to 0x0f for CMOS sensor</t>
-  </si>
-  <si>
-    <t>set quick look mode and photon counting mode exposure time to 0x10 for CMOS sensor</t>
-  </si>
-  <si>
-    <t>set quick look mode and photon counting mode exposure time to 0x11 for CMOS sensor</t>
-  </si>
-  <si>
-    <t>set quick look mode and photon counting mode exposure time to 0x12 for CMOS sensor</t>
-  </si>
-  <si>
-    <t>set quick look mode and photon counting mode exposure time to 0x13 for CMOS sensor</t>
-  </si>
-  <si>
-    <t>set quick look mode and photon counting mode exposure time to 0x14 for CMOS sensor</t>
-  </si>
-  <si>
-    <t>set quick look mode and photon counting mode exposure time to 0x15 for CMOS sensor</t>
-  </si>
-  <si>
-    <t>set quick look mode and photon counting mode exposure time to 0x16 for CMOS sensor</t>
-  </si>
-  <si>
-    <t>set quick look mode and photon counting mode exposure time to 0x17 for CMOS sensor</t>
-  </si>
-  <si>
-    <t>set quick look mode and photon counting mode exposure time to 0x18 for CMOS sensor</t>
-  </si>
-  <si>
-    <t>set quick look mode and photon counting mode exposure time to 0x19 for CMOS sensor</t>
-  </si>
-  <si>
-    <t>set quick look mode and photon counting mode exposure time to 0x1a for CMOS sensor</t>
-  </si>
-  <si>
-    <t>set quick look mode and photon counting mode exposure time to 0x1b for CMOS sensor</t>
-  </si>
-  <si>
-    <t>set quick look mode and photon counting mode exposure time to 0x1c for CMOS sensor</t>
-  </si>
-  <si>
-    <t>set quick look mode and photon counting mode exposure time to 0x1d for CMOS sensor</t>
-  </si>
-  <si>
-    <t>set quick look mode and photon counting mode exposure time to 0x1e for CMOS sensor</t>
-  </si>
-  <si>
-    <t>set quick look mode and photon counting mode exposure time to 0x1f for CMOS sensor</t>
-  </si>
-  <si>
-    <t>set quick look mode and photon counting mode exposure time to 0x20 for CMOS sensor</t>
-  </si>
-  <si>
-    <t>set quick look mode and photon counting mode exposure time to 0x21 for CMOS sensor</t>
-  </si>
-  <si>
     <t>cmos_stop_to_start</t>
   </si>
   <si>
@@ -937,6 +691,243 @@
   </si>
   <si>
     <t>deletes all stored image data</t>
+  </si>
+  <si>
+    <t>set_exposure_slot_00</t>
+  </si>
+  <si>
+    <t>set_exposure_slot_01</t>
+  </si>
+  <si>
+    <t>set_exposure_slot_02</t>
+  </si>
+  <si>
+    <t>set_exposure_slot_03</t>
+  </si>
+  <si>
+    <t>set_exposure_slot_04</t>
+  </si>
+  <si>
+    <t>set_exposure_slot_05</t>
+  </si>
+  <si>
+    <t>set_exposure_slot_06</t>
+  </si>
+  <si>
+    <t>set_exposure_slot_07</t>
+  </si>
+  <si>
+    <t>set_exposure_slot_08</t>
+  </si>
+  <si>
+    <t>set_exposure_slot_09</t>
+  </si>
+  <si>
+    <t>set_exposure_slot_10</t>
+  </si>
+  <si>
+    <t>set_exposure_slot_11</t>
+  </si>
+  <si>
+    <t>set_exposure_slot_12</t>
+  </si>
+  <si>
+    <t>set_exposure_slot_13</t>
+  </si>
+  <si>
+    <t>set_exposure_slot_14</t>
+  </si>
+  <si>
+    <t>set_exposure_slot_15</t>
+  </si>
+  <si>
+    <t>set_exposure_slot_16</t>
+  </si>
+  <si>
+    <t>set_exposure_slot_17</t>
+  </si>
+  <si>
+    <t>set_exposure_slot_18</t>
+  </si>
+  <si>
+    <t>set_exposure_slot_19</t>
+  </si>
+  <si>
+    <t>set_exposure_slot_20</t>
+  </si>
+  <si>
+    <t>set_exposure_slot_21</t>
+  </si>
+  <si>
+    <t>set_exposure_slot_22</t>
+  </si>
+  <si>
+    <t>set_exposure_slot_23</t>
+  </si>
+  <si>
+    <t>set_exposure_slot_24</t>
+  </si>
+  <si>
+    <t>set_exposure_slot_25</t>
+  </si>
+  <si>
+    <t>set_exposure_slot_26</t>
+  </si>
+  <si>
+    <t>set_exposure_slot_27</t>
+  </si>
+  <si>
+    <t>set_exposure_slot_28</t>
+  </si>
+  <si>
+    <t>set_exposure_slot_29</t>
+  </si>
+  <si>
+    <t>set_exposure_slot_30</t>
+  </si>
+  <si>
+    <t>set_exposure_slot_31</t>
+  </si>
+  <si>
+    <t>0xc01085f0</t>
+  </si>
+  <si>
+    <t>0xa91085f0</t>
+  </si>
+  <si>
+    <t>0x931085f0</t>
+  </si>
+  <si>
+    <t>0x801085f0</t>
+  </si>
+  <si>
+    <t>0x6f1085f0</t>
+  </si>
+  <si>
+    <t>0x611085f0</t>
+  </si>
+  <si>
+    <t>0x541085f0</t>
+  </si>
+  <si>
+    <t>0x491085f0</t>
+  </si>
+  <si>
+    <t>0x401085f0</t>
+  </si>
+  <si>
+    <t>0x371085f0</t>
+  </si>
+  <si>
+    <t>0x301085f0</t>
+  </si>
+  <si>
+    <t>0x2a1085f0</t>
+  </si>
+  <si>
+    <t>0x241085f0</t>
+  </si>
+  <si>
+    <t>0x001085f0</t>
+  </si>
+  <si>
+    <t>0x08</t>
+  </si>
+  <si>
+    <t>0x7d</t>
+  </si>
+  <si>
+    <t>set quick look mode and photon counting mode inttim to 192 for CMOS sensor</t>
+  </si>
+  <si>
+    <t>set quick look mode and photon counting mode inttim to 169 for CMOS sensor</t>
+  </si>
+  <si>
+    <t>set quick look mode and photon counting mode inttim to 147 for CMOS sensor</t>
+  </si>
+  <si>
+    <t>set quick look mode and photon counting mode inttim to 128 for CMOS sensor</t>
+  </si>
+  <si>
+    <t>set quick look mode and photon counting mode inttim to 111 for CMOS sensor</t>
+  </si>
+  <si>
+    <t>set quick look mode and photon counting mode inttim to 97 for CMOS sensor</t>
+  </si>
+  <si>
+    <t>set quick look mode and photon counting mode inttim to 84 for CMOS sensor</t>
+  </si>
+  <si>
+    <t>set quick look mode and photon counting mode inttim to 73 for CMOS sensor</t>
+  </si>
+  <si>
+    <t>set quick look mode and photon counting mode inttim to 64 for CMOS sensor</t>
+  </si>
+  <si>
+    <t>set quick look mode and photon counting mode inttim to 55 for CMOS sensor</t>
+  </si>
+  <si>
+    <t>set quick look mode and photon counting mode inttim to 48 for CMOS sensor</t>
+  </si>
+  <si>
+    <t>set quick look mode and photon counting mode inttim to 42 for CMOS sensor</t>
+  </si>
+  <si>
+    <t>set quick look mode and photon counting mode inttim to 36 for CMOS sensor</t>
+  </si>
+  <si>
+    <t>set quick look mode and photon counting mode inttim to 31 for CMOS sensor</t>
+  </si>
+  <si>
+    <t>set quick look mode and photon counting mode inttim to 27 for CMOS sensor</t>
+  </si>
+  <si>
+    <t>set quick look mode and photon counting mode inttim to 24 for CMOS sensor</t>
+  </si>
+  <si>
+    <t>set quick look mode and photon counting mode inttim to 20 for CMOS sensor</t>
+  </si>
+  <si>
+    <t>set quick look mode and photon counting mode inttim to 18 for CMOS sensor</t>
+  </si>
+  <si>
+    <t>set quick look mode and photon counting mode inttim to 15 for CMOS sensor</t>
+  </si>
+  <si>
+    <t>set quick look mode and photon counting mode inttim to 13 for CMOS sensor</t>
+  </si>
+  <si>
+    <t>set quick look mode and photon counting mode inttim to 11 for CMOS sensor</t>
+  </si>
+  <si>
+    <t>set quick look mode and photon counting mode inttim to 10 for CMOS sensor</t>
+  </si>
+  <si>
+    <t>set quick look mode and photon counting mode inttim to 8 for CMOS sensor</t>
+  </si>
+  <si>
+    <t>set quick look mode and photon counting mode inttim to 7 for CMOS sensor</t>
+  </si>
+  <si>
+    <t>set quick look mode and photon counting mode inttim to 6 for CMOS sensor</t>
+  </si>
+  <si>
+    <t>set quick look mode and photon counting mode inttim to 5 for CMOS sensor</t>
+  </si>
+  <si>
+    <t>set quick look mode and photon counting mode inttim to 4 for CMOS sensor</t>
+  </si>
+  <si>
+    <t>set quick look mode and photon counting mode inttim to 3 for CMOS sensor</t>
+  </si>
+  <si>
+    <t>set quick look mode and photon counting mode inttim to 2 for CMOS sensor</t>
+  </si>
+  <si>
+    <t>set quick look mode and photon counting mode inttim to 1 for CMOS sensor</t>
+  </si>
+  <si>
+    <t>set quick look mode and photon counting mode inttim to 0 for CMOS sensor</t>
   </si>
 </sst>
 </file>
@@ -1439,10 +1430,10 @@
   <dimension ref="A1:AC85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B55" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="E32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E45" sqref="E45"/>
+      <selection pane="bottomRight" activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -1899,7 +1890,7 @@
         <v>44</v>
       </c>
       <c r="K6" s="23" t="s">
-        <v>296</v>
+        <v>214</v>
       </c>
       <c r="L6" s="6">
         <v>0</v>
@@ -1944,7 +1935,7 @@
         <v>74</v>
       </c>
       <c r="Z6" s="3" t="s">
-        <v>295</v>
+        <v>213</v>
       </c>
       <c r="AA6" s="25" t="s">
         <v>41</v>
@@ -4357,7 +4348,7 @@
         <v>17</v>
       </c>
       <c r="K34" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L34" s="6">
         <v>1</v>
@@ -4399,7 +4390,7 @@
         <v>68</v>
       </c>
       <c r="Y34" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z34" s="3" t="s">
         <v>41</v>
@@ -4447,7 +4438,7 @@
         <v>17</v>
       </c>
       <c r="K35" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L35" s="6">
         <v>1</v>
@@ -4489,7 +4480,7 @@
         <v>68</v>
       </c>
       <c r="Y35" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z35" s="3" t="s">
         <v>41</v>
@@ -4537,7 +4528,7 @@
         <v>17</v>
       </c>
       <c r="K36" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L36" s="6">
         <v>0</v>
@@ -4579,7 +4570,7 @@
         <v>68</v>
       </c>
       <c r="Y36" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z36" s="3" t="s">
         <v>87</v>
@@ -4627,7 +4618,7 @@
         <v>17</v>
       </c>
       <c r="K37" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L37" s="6">
         <v>0</v>
@@ -4669,7 +4660,7 @@
         <v>68</v>
       </c>
       <c r="Y37" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z37" s="3" t="s">
         <v>88</v>
@@ -4717,7 +4708,7 @@
         <v>17</v>
       </c>
       <c r="K38" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L38" s="6">
         <v>0</v>
@@ -4759,7 +4750,7 @@
         <v>68</v>
       </c>
       <c r="Y38" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z38" s="3" t="s">
         <v>89</v>
@@ -4807,7 +4798,7 @@
         <v>17</v>
       </c>
       <c r="K39" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L39" s="6">
         <v>0</v>
@@ -4849,7 +4840,7 @@
         <v>68</v>
       </c>
       <c r="Y39" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z39" s="3" t="s">
         <v>41</v>
@@ -4897,7 +4888,7 @@
         <v>17</v>
       </c>
       <c r="K40" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L40" s="6">
         <v>0</v>
@@ -4939,7 +4930,7 @@
         <v>68</v>
       </c>
       <c r="Y40" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z40" s="3" t="s">
         <v>90</v>
@@ -4987,7 +4978,7 @@
         <v>17</v>
       </c>
       <c r="K41" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L41" s="6">
         <v>0</v>
@@ -5029,7 +5020,7 @@
         <v>68</v>
       </c>
       <c r="Y41" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z41" s="3" t="s">
         <v>91</v>
@@ -5046,7 +5037,7 @@
     </row>
     <row r="42" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="19" t="s">
-        <v>290</v>
+        <v>208</v>
       </c>
       <c r="B42" s="18" t="s">
         <v>55</v>
@@ -5077,7 +5068,7 @@
         <v>17</v>
       </c>
       <c r="K42" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L42" s="6">
         <v>0</v>
@@ -5119,10 +5110,10 @@
         <v>68</v>
       </c>
       <c r="Y42" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z42" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AA42" s="23" t="s">
         <v>113</v>
@@ -5131,7 +5122,7 @@
         <v>70</v>
       </c>
       <c r="AC42" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="43" spans="1:29" ht="16" x14ac:dyDescent="0.2">
@@ -5167,7 +5158,7 @@
         <v>17</v>
       </c>
       <c r="K43" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L43" s="6">
         <v>0</v>
@@ -5209,7 +5200,7 @@
         <v>68</v>
       </c>
       <c r="Y43" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z43" s="3" t="s">
         <v>185</v>
@@ -5221,7 +5212,7 @@
         <v>70</v>
       </c>
       <c r="AC43" t="s">
-        <v>298</v>
+        <v>216</v>
       </c>
     </row>
     <row r="44" spans="1:29" ht="16" x14ac:dyDescent="0.2">
@@ -5257,7 +5248,7 @@
         <v>17</v>
       </c>
       <c r="K44" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L44" s="6">
         <v>0</v>
@@ -5299,7 +5290,7 @@
         <v>68</v>
       </c>
       <c r="Y44" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z44" s="3" t="s">
         <v>186</v>
@@ -5311,12 +5302,12 @@
         <v>70</v>
       </c>
       <c r="AC44" t="s">
-        <v>297</v>
+        <v>215</v>
       </c>
     </row>
     <row r="45" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="19" t="s">
-        <v>291</v>
+        <v>209</v>
       </c>
       <c r="B45" s="18" t="s">
         <v>55</v>
@@ -5347,7 +5338,7 @@
         <v>17</v>
       </c>
       <c r="K45" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L45" s="6">
         <v>0</v>
@@ -5389,10 +5380,10 @@
         <v>68</v>
       </c>
       <c r="Y45" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z45" s="3" t="s">
-        <v>293</v>
+        <v>211</v>
       </c>
       <c r="AA45" s="23" t="s">
         <v>113</v>
@@ -5401,12 +5392,12 @@
         <v>70</v>
       </c>
       <c r="AC45" t="s">
-        <v>299</v>
+        <v>217</v>
       </c>
     </row>
     <row r="46" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="19" t="s">
-        <v>292</v>
+        <v>210</v>
       </c>
       <c r="B46" s="18" t="s">
         <v>55</v>
@@ -5437,7 +5428,7 @@
         <v>17</v>
       </c>
       <c r="K46" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L46" s="6">
         <v>0</v>
@@ -5479,10 +5470,10 @@
         <v>68</v>
       </c>
       <c r="Y46" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z46" s="3" t="s">
-        <v>294</v>
+        <v>212</v>
       </c>
       <c r="AA46" s="23" t="s">
         <v>113</v>
@@ -5491,12 +5482,12 @@
         <v>70</v>
       </c>
       <c r="AC46" t="s">
-        <v>300</v>
+        <v>218</v>
       </c>
     </row>
     <row r="47" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B47" s="18" t="s">
         <v>55</v>
@@ -5527,7 +5518,7 @@
         <v>17</v>
       </c>
       <c r="K47" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L47" s="6">
         <v>0</v>
@@ -5569,10 +5560,10 @@
         <v>68</v>
       </c>
       <c r="Y47" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z47" s="3" t="s">
-        <v>224</v>
+        <v>190</v>
       </c>
       <c r="AA47" s="23" t="s">
         <v>113</v>
@@ -5581,12 +5572,12 @@
         <v>70</v>
       </c>
       <c r="AC47" t="s">
-        <v>223</v>
+        <v>267</v>
       </c>
     </row>
     <row r="48" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="19" t="s">
-        <v>191</v>
+        <v>219</v>
       </c>
       <c r="B48" s="18" t="s">
         <v>55</v>
@@ -5617,7 +5608,7 @@
         <v>17</v>
       </c>
       <c r="K48" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L48" s="30">
         <v>0</v>
@@ -5659,24 +5650,24 @@
         <v>68</v>
       </c>
       <c r="Y48" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z48" s="3" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="AA48" s="23" t="s">
-        <v>226</v>
+        <v>251</v>
       </c>
       <c r="AB48" t="s">
         <v>70</v>
       </c>
       <c r="AC48" t="s">
-        <v>227</v>
+        <v>267</v>
       </c>
     </row>
     <row r="49" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="19" t="s">
-        <v>192</v>
+        <v>220</v>
       </c>
       <c r="B49" s="18" t="s">
         <v>55</v>
@@ -5707,7 +5698,7 @@
         <v>17</v>
       </c>
       <c r="K49" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L49" s="30">
         <v>0</v>
@@ -5749,24 +5740,24 @@
         <v>68</v>
       </c>
       <c r="Y49" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z49" s="3" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="AA49" s="23" t="s">
-        <v>232</v>
+        <v>252</v>
       </c>
       <c r="AB49" t="s">
         <v>70</v>
       </c>
       <c r="AC49" t="s">
-        <v>228</v>
+        <v>268</v>
       </c>
     </row>
     <row r="50" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="19" t="s">
-        <v>193</v>
+        <v>221</v>
       </c>
       <c r="B50" s="18" t="s">
         <v>55</v>
@@ -5797,7 +5788,7 @@
         <v>17</v>
       </c>
       <c r="K50" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L50" s="30">
         <v>0</v>
@@ -5839,24 +5830,24 @@
         <v>68</v>
       </c>
       <c r="Y50" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z50" s="27" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="AA50" s="23" t="s">
-        <v>233</v>
+        <v>253</v>
       </c>
       <c r="AB50" t="s">
         <v>70</v>
       </c>
       <c r="AC50" t="s">
-        <v>229</v>
+        <v>269</v>
       </c>
     </row>
     <row r="51" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="19" t="s">
-        <v>194</v>
+        <v>222</v>
       </c>
       <c r="B51" s="18" t="s">
         <v>55</v>
@@ -5887,7 +5878,7 @@
         <v>17</v>
       </c>
       <c r="K51" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L51" s="30">
         <v>0</v>
@@ -5929,24 +5920,24 @@
         <v>68</v>
       </c>
       <c r="Y51" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z51" s="3" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="AA51" s="23" t="s">
-        <v>234</v>
+        <v>254</v>
       </c>
       <c r="AB51" t="s">
         <v>70</v>
       </c>
       <c r="AC51" t="s">
-        <v>230</v>
+        <v>270</v>
       </c>
     </row>
     <row r="52" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="19" t="s">
-        <v>195</v>
+        <v>223</v>
       </c>
       <c r="B52" s="18" t="s">
         <v>55</v>
@@ -5977,7 +5968,7 @@
         <v>17</v>
       </c>
       <c r="K52" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L52" s="30">
         <v>0</v>
@@ -6019,24 +6010,24 @@
         <v>68</v>
       </c>
       <c r="Y52" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z52" s="27" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="AA52" s="25" t="s">
-        <v>235</v>
+        <v>255</v>
       </c>
       <c r="AB52" t="s">
         <v>70</v>
       </c>
       <c r="AC52" t="s">
-        <v>231</v>
+        <v>271</v>
       </c>
     </row>
     <row r="53" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="19" t="s">
-        <v>196</v>
+        <v>224</v>
       </c>
       <c r="B53" s="18" t="s">
         <v>55</v>
@@ -6067,7 +6058,7 @@
         <v>17</v>
       </c>
       <c r="K53" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L53" s="30">
         <v>0</v>
@@ -6109,24 +6100,24 @@
         <v>68</v>
       </c>
       <c r="Y53" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z53" s="3" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="AA53" s="25" t="s">
-        <v>236</v>
+        <v>256</v>
       </c>
       <c r="AB53" t="s">
         <v>70</v>
       </c>
       <c r="AC53" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
     </row>
     <row r="54" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="19" t="s">
-        <v>197</v>
+        <v>225</v>
       </c>
       <c r="B54" s="18" t="s">
         <v>55</v>
@@ -6157,7 +6148,7 @@
         <v>17</v>
       </c>
       <c r="K54" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L54" s="30">
         <v>0</v>
@@ -6199,24 +6190,24 @@
         <v>68</v>
       </c>
       <c r="Y54" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z54" s="27" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="AA54" s="25" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="AB54" t="s">
         <v>70</v>
       </c>
       <c r="AC54" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
     </row>
     <row r="55" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="19" t="s">
-        <v>198</v>
+        <v>226</v>
       </c>
       <c r="B55" s="18" t="s">
         <v>55</v>
@@ -6247,7 +6238,7 @@
         <v>17</v>
       </c>
       <c r="K55" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L55" s="30">
         <v>0</v>
@@ -6289,24 +6280,24 @@
         <v>68</v>
       </c>
       <c r="Y55" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z55" s="3" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="AA55" s="25" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
       <c r="AB55" t="s">
         <v>70</v>
       </c>
       <c r="AC55" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
     </row>
     <row r="56" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="19" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
       <c r="B56" s="18" t="s">
         <v>55</v>
@@ -6337,7 +6328,7 @@
         <v>17</v>
       </c>
       <c r="K56" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L56" s="30">
         <v>0</v>
@@ -6379,24 +6370,24 @@
         <v>68</v>
       </c>
       <c r="Y56" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z56" s="27" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="AA56" s="25" t="s">
-        <v>239</v>
+        <v>259</v>
       </c>
       <c r="AB56" t="s">
         <v>70</v>
       </c>
       <c r="AC56" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
     </row>
     <row r="57" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="19" t="s">
-        <v>212</v>
+        <v>228</v>
       </c>
       <c r="B57" s="18" t="s">
         <v>55</v>
@@ -6427,7 +6418,7 @@
         <v>17</v>
       </c>
       <c r="K57" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L57" s="30">
         <v>0</v>
@@ -6469,24 +6460,24 @@
         <v>68</v>
       </c>
       <c r="Y57" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z57" s="3" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="AA57" s="25" t="s">
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="AB57" t="s">
         <v>70</v>
       </c>
       <c r="AC57" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
     </row>
     <row r="58" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="19" t="s">
-        <v>213</v>
+        <v>229</v>
       </c>
       <c r="B58" s="18" t="s">
         <v>55</v>
@@ -6517,7 +6508,7 @@
         <v>17</v>
       </c>
       <c r="K58" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L58" s="30">
         <v>0</v>
@@ -6559,24 +6550,24 @@
         <v>68</v>
       </c>
       <c r="Y58" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z58" s="27" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="AA58" s="23" t="s">
-        <v>241</v>
+        <v>261</v>
       </c>
       <c r="AB58" t="s">
         <v>70</v>
       </c>
       <c r="AC58" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
     </row>
     <row r="59" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="19" t="s">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="B59" s="18" t="s">
         <v>55</v>
@@ -6607,7 +6598,7 @@
         <v>17</v>
       </c>
       <c r="K59" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L59" s="30">
         <v>0</v>
@@ -6649,24 +6640,24 @@
         <v>68</v>
       </c>
       <c r="Y59" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z59" s="3" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="AA59" s="25" t="s">
-        <v>242</v>
+        <v>262</v>
       </c>
       <c r="AB59" t="s">
         <v>70</v>
       </c>
       <c r="AC59" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
     </row>
     <row r="60" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="19" t="s">
-        <v>215</v>
+        <v>231</v>
       </c>
       <c r="B60" s="18" t="s">
         <v>55</v>
@@ -6697,7 +6688,7 @@
         <v>17</v>
       </c>
       <c r="K60" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L60" s="30">
         <v>0</v>
@@ -6739,24 +6730,24 @@
         <v>68</v>
       </c>
       <c r="Y60" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z60" s="27" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="AA60" s="25" t="s">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="AB60" t="s">
         <v>70</v>
       </c>
       <c r="AC60" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
     </row>
     <row r="61" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="19" t="s">
-        <v>216</v>
+        <v>232</v>
       </c>
       <c r="B61" s="18" t="s">
         <v>55</v>
@@ -6787,7 +6778,7 @@
         <v>17</v>
       </c>
       <c r="K61" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L61" s="30">
         <v>0</v>
@@ -6829,24 +6820,24 @@
         <v>68</v>
       </c>
       <c r="Y61" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z61" s="3" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="AA61" s="25" t="s">
-        <v>244</v>
+        <v>207</v>
       </c>
       <c r="AB61" t="s">
         <v>70</v>
       </c>
       <c r="AC61" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
     </row>
     <row r="62" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="19" t="s">
-        <v>199</v>
+        <v>233</v>
       </c>
       <c r="B62" s="18" t="s">
         <v>55</v>
@@ -6877,7 +6868,7 @@
         <v>17</v>
       </c>
       <c r="K62" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L62" s="30">
         <v>0</v>
@@ -6919,24 +6910,24 @@
         <v>68</v>
       </c>
       <c r="Y62" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z62" s="27" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="AA62" s="23" t="s">
-        <v>246</v>
+        <v>206</v>
       </c>
       <c r="AB62" t="s">
         <v>70</v>
       </c>
       <c r="AC62" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
     </row>
     <row r="63" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="19" t="s">
-        <v>200</v>
+        <v>234</v>
       </c>
       <c r="B63" s="18" t="s">
         <v>55</v>
@@ -6967,7 +6958,7 @@
         <v>17</v>
       </c>
       <c r="K63" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L63" s="30">
         <v>0</v>
@@ -7009,24 +7000,24 @@
         <v>68</v>
       </c>
       <c r="Y63" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z63" s="3" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="AA63" s="23" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
       <c r="AB63" t="s">
         <v>70</v>
       </c>
       <c r="AC63" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
     </row>
     <row r="64" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="19" t="s">
-        <v>201</v>
+        <v>235</v>
       </c>
       <c r="B64" s="18" t="s">
         <v>55</v>
@@ -7057,7 +7048,7 @@
         <v>17</v>
       </c>
       <c r="K64" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L64" s="30">
         <v>0</v>
@@ -7099,24 +7090,24 @@
         <v>68</v>
       </c>
       <c r="Y64" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z64" s="27" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="AA64" s="25" t="s">
-        <v>247</v>
+        <v>204</v>
       </c>
       <c r="AB64" t="s">
         <v>70</v>
       </c>
       <c r="AC64" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
     </row>
     <row r="65" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="19" t="s">
-        <v>202</v>
+        <v>236</v>
       </c>
       <c r="B65" s="18" t="s">
         <v>55</v>
@@ -7147,7 +7138,7 @@
         <v>17</v>
       </c>
       <c r="K65" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L65" s="30">
         <v>0</v>
@@ -7189,24 +7180,24 @@
         <v>68</v>
       </c>
       <c r="Y65" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z65" s="3" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="AA65" s="25" t="s">
-        <v>248</v>
+        <v>203</v>
       </c>
       <c r="AB65" t="s">
         <v>70</v>
       </c>
       <c r="AC65" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
     </row>
     <row r="66" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="19" t="s">
-        <v>203</v>
+        <v>237</v>
       </c>
       <c r="B66" s="18" t="s">
         <v>55</v>
@@ -7237,7 +7228,7 @@
         <v>17</v>
       </c>
       <c r="K66" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L66" s="30">
         <v>0</v>
@@ -7279,24 +7270,24 @@
         <v>68</v>
       </c>
       <c r="Y66" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z66" s="27" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="AA66" s="25" t="s">
-        <v>249</v>
+        <v>202</v>
       </c>
       <c r="AB66" t="s">
         <v>70</v>
       </c>
       <c r="AC66" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
     </row>
     <row r="67" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="19" t="s">
-        <v>204</v>
+        <v>238</v>
       </c>
       <c r="B67" s="18" t="s">
         <v>55</v>
@@ -7327,7 +7318,7 @@
         <v>17</v>
       </c>
       <c r="K67" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L67" s="30">
         <v>0</v>
@@ -7369,24 +7360,24 @@
         <v>68</v>
       </c>
       <c r="Y67" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z67" s="3" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="AA67" s="25" t="s">
-        <v>250</v>
+        <v>201</v>
       </c>
       <c r="AB67" t="s">
         <v>70</v>
       </c>
       <c r="AC67" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
     </row>
     <row r="68" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="19" t="s">
-        <v>205</v>
+        <v>239</v>
       </c>
       <c r="B68" s="18" t="s">
         <v>55</v>
@@ -7417,7 +7408,7 @@
         <v>17</v>
       </c>
       <c r="K68" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L68" s="30">
         <v>0</v>
@@ -7459,24 +7450,24 @@
         <v>68</v>
       </c>
       <c r="Y68" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z68" s="27" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="AA68" s="25" t="s">
-        <v>251</v>
+        <v>200</v>
       </c>
       <c r="AB68" t="s">
         <v>70</v>
       </c>
       <c r="AC68" t="s">
-        <v>278</v>
+        <v>287</v>
       </c>
     </row>
     <row r="69" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="19" t="s">
-        <v>206</v>
+        <v>240</v>
       </c>
       <c r="B69" s="18" t="s">
         <v>55</v>
@@ -7507,7 +7498,7 @@
         <v>17</v>
       </c>
       <c r="K69" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L69" s="30">
         <v>0</v>
@@ -7549,24 +7540,24 @@
         <v>68</v>
       </c>
       <c r="Y69" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z69" s="3" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="AA69" s="25" t="s">
-        <v>252</v>
+        <v>199</v>
       </c>
       <c r="AB69" t="s">
         <v>70</v>
       </c>
       <c r="AC69" t="s">
-        <v>279</v>
+        <v>288</v>
       </c>
     </row>
     <row r="70" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="19" t="s">
-        <v>207</v>
+        <v>241</v>
       </c>
       <c r="B70" s="18" t="s">
         <v>55</v>
@@ -7597,7 +7588,7 @@
         <v>17</v>
       </c>
       <c r="K70" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L70" s="30">
         <v>0</v>
@@ -7639,24 +7630,24 @@
         <v>68</v>
       </c>
       <c r="Y70" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z70" s="27" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="AA70" s="25" t="s">
-        <v>253</v>
+        <v>198</v>
       </c>
       <c r="AB70" t="s">
         <v>70</v>
       </c>
       <c r="AC70" t="s">
-        <v>280</v>
+        <v>289</v>
       </c>
     </row>
     <row r="71" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="19" t="s">
-        <v>208</v>
+        <v>242</v>
       </c>
       <c r="B71" s="18" t="s">
         <v>55</v>
@@ -7687,7 +7678,7 @@
         <v>17</v>
       </c>
       <c r="K71" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L71" s="30">
         <v>0</v>
@@ -7729,24 +7720,24 @@
         <v>68</v>
       </c>
       <c r="Y71" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z71" s="3" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="AA71" s="25" t="s">
-        <v>254</v>
+        <v>197</v>
       </c>
       <c r="AB71" t="s">
         <v>70</v>
       </c>
       <c r="AC71" t="s">
-        <v>281</v>
+        <v>290</v>
       </c>
     </row>
     <row r="72" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="19" t="s">
-        <v>217</v>
+        <v>243</v>
       </c>
       <c r="B72" s="18" t="s">
         <v>55</v>
@@ -7777,7 +7768,7 @@
         <v>17</v>
       </c>
       <c r="K72" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L72" s="30">
         <v>0</v>
@@ -7819,24 +7810,24 @@
         <v>68</v>
       </c>
       <c r="Y72" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z72" s="27" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="AA72" s="25" t="s">
-        <v>255</v>
+        <v>196</v>
       </c>
       <c r="AB72" t="s">
         <v>70</v>
       </c>
       <c r="AC72" t="s">
-        <v>282</v>
+        <v>291</v>
       </c>
     </row>
     <row r="73" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="19" t="s">
-        <v>218</v>
+        <v>244</v>
       </c>
       <c r="B73" s="18" t="s">
         <v>55</v>
@@ -7867,7 +7858,7 @@
         <v>17</v>
       </c>
       <c r="K73" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L73" s="30">
         <v>0</v>
@@ -7909,24 +7900,24 @@
         <v>68</v>
       </c>
       <c r="Y73" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z73" s="3" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="AA73" s="25" t="s">
-        <v>256</v>
+        <v>195</v>
       </c>
       <c r="AB73" t="s">
         <v>70</v>
       </c>
       <c r="AC73" t="s">
-        <v>283</v>
+        <v>292</v>
       </c>
     </row>
     <row r="74" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="19" t="s">
-        <v>219</v>
+        <v>245</v>
       </c>
       <c r="B74" s="18" t="s">
         <v>55</v>
@@ -7957,7 +7948,7 @@
         <v>17</v>
       </c>
       <c r="K74" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L74" s="30">
         <v>0</v>
@@ -7999,24 +7990,24 @@
         <v>68</v>
       </c>
       <c r="Y74" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z74" s="27" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="AA74" s="25" t="s">
-        <v>257</v>
+        <v>194</v>
       </c>
       <c r="AB74" t="s">
         <v>70</v>
       </c>
       <c r="AC74" t="s">
-        <v>284</v>
+        <v>293</v>
       </c>
     </row>
     <row r="75" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="19" t="s">
-        <v>220</v>
+        <v>246</v>
       </c>
       <c r="B75" s="18" t="s">
         <v>55</v>
@@ -8047,7 +8038,7 @@
         <v>17</v>
       </c>
       <c r="K75" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L75" s="30">
         <v>0</v>
@@ -8089,24 +8080,24 @@
         <v>68</v>
       </c>
       <c r="Y75" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z75" s="3" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="AA75" s="25" t="s">
-        <v>258</v>
+        <v>193</v>
       </c>
       <c r="AB75" t="s">
         <v>70</v>
       </c>
       <c r="AC75" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
     </row>
     <row r="76" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="19" t="s">
-        <v>221</v>
+        <v>247</v>
       </c>
       <c r="B76" s="18" t="s">
         <v>55</v>
@@ -8137,7 +8128,7 @@
         <v>17</v>
       </c>
       <c r="K76" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L76" s="30">
         <v>0</v>
@@ -8179,24 +8170,24 @@
         <v>68</v>
       </c>
       <c r="Y76" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z76" s="27" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="AA76" s="25" t="s">
-        <v>259</v>
+        <v>192</v>
       </c>
       <c r="AB76" t="s">
         <v>70</v>
       </c>
       <c r="AC76" t="s">
-        <v>286</v>
+        <v>295</v>
       </c>
     </row>
     <row r="77" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="19" t="s">
-        <v>222</v>
+        <v>248</v>
       </c>
       <c r="B77" s="18" t="s">
         <v>55</v>
@@ -8227,7 +8218,7 @@
         <v>17</v>
       </c>
       <c r="K77" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L77" s="30">
         <v>0</v>
@@ -8269,24 +8260,24 @@
         <v>68</v>
       </c>
       <c r="Y77" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z77" s="3" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="AA77" s="25" t="s">
-        <v>260</v>
+        <v>113</v>
       </c>
       <c r="AB77" t="s">
         <v>70</v>
       </c>
       <c r="AC77" t="s">
-        <v>287</v>
+        <v>296</v>
       </c>
     </row>
     <row r="78" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="19" t="s">
-        <v>209</v>
+        <v>249</v>
       </c>
       <c r="B78" s="18" t="s">
         <v>55</v>
@@ -8317,7 +8308,7 @@
         <v>17</v>
       </c>
       <c r="K78" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L78" s="30">
         <v>0</v>
@@ -8359,24 +8350,24 @@
         <v>68</v>
       </c>
       <c r="Y78" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z78" s="27" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="AA78" s="23" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="AB78" t="s">
         <v>70</v>
       </c>
       <c r="AC78" t="s">
-        <v>288</v>
+        <v>297</v>
       </c>
     </row>
     <row r="79" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="19" t="s">
-        <v>210</v>
+        <v>250</v>
       </c>
       <c r="B79" s="18" t="s">
         <v>55</v>
@@ -8407,7 +8398,7 @@
         <v>17</v>
       </c>
       <c r="K79" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L79" s="30">
         <v>0</v>
@@ -8449,19 +8440,19 @@
         <v>68</v>
       </c>
       <c r="Y79" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z79" s="3" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="AA79" s="23" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="AB79" t="s">
         <v>70</v>
       </c>
       <c r="AC79" t="s">
-        <v>289</v>
+        <v>297</v>
       </c>
     </row>
     <row r="80" spans="1:29" ht="16" x14ac:dyDescent="0.2">
@@ -8497,7 +8488,7 @@
         <v>17</v>
       </c>
       <c r="K80" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L80" s="6">
         <v>0</v>
@@ -8539,7 +8530,7 @@
         <v>68</v>
       </c>
       <c r="Y80" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z80" s="3" t="s">
         <v>119</v>
@@ -8587,7 +8578,7 @@
         <v>17</v>
       </c>
       <c r="K81" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L81" s="6">
         <v>0</v>
@@ -8629,7 +8620,7 @@
         <v>68</v>
       </c>
       <c r="Y81" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z81" s="3" t="s">
         <v>118</v>
@@ -8677,7 +8668,7 @@
         <v>17</v>
       </c>
       <c r="K82" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L82" s="6">
         <v>0</v>
@@ -8719,7 +8710,7 @@
         <v>68</v>
       </c>
       <c r="Y82" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z82" s="3" t="s">
         <v>117</v>
@@ -8767,7 +8758,7 @@
         <v>17</v>
       </c>
       <c r="K83" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L83" s="6">
         <v>0</v>
@@ -8809,7 +8800,7 @@
         <v>68</v>
       </c>
       <c r="Y83" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z83" s="3" t="s">
         <v>116</v>
@@ -8857,7 +8848,7 @@
         <v>17</v>
       </c>
       <c r="K84" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L84" s="6">
         <v>0</v>
@@ -8899,7 +8890,7 @@
         <v>68</v>
       </c>
       <c r="Y84" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z84" s="3" t="s">
         <v>115</v>
@@ -8947,7 +8938,7 @@
         <v>17</v>
       </c>
       <c r="K85" s="23" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="L85" s="6">
         <v>0</v>
@@ -8989,7 +8980,7 @@
         <v>68</v>
       </c>
       <c r="Y85" s="22" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="Z85" s="3" t="s">
         <v>114</v>

</xml_diff>

<commit_message>
adding intercept commands for Housekeeping (formatter), adding vth+dth commands for CdTe DE
</commit_message>
<xml_diff>
--- a/commands/cmos1/cmos1_command_deck.xlsx
+++ b/commands/cmos1/cmos1_command_deck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi-4matter/foxsi4-commands/commands/cmos1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66346D7-8988-D74D-99E7-F5014444A5CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E9701B2-62F4-8C41-A3EE-F92FA573F3CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="760" windowWidth="30220" windowHeight="17880" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
@@ -1433,7 +1433,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="E32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A79" sqref="A79"/>
+      <selection pane="bottomRight" activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>

</xml_diff>